<commit_message>
Finished interim update on affordable projects for Carol and Carolina
</commit_message>
<xml_diff>
--- a/analysis/Output/aff_tests.xlsx
+++ b/analysis/Output/aff_tests.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="36720" yWindow="3620" windowWidth="25600" windowHeight="16080" tabRatio="500"/>
+    <workbookView xWindow="31140" yWindow="3020" windowWidth="25600" windowHeight="15500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
   <si>
     <t>Entitlement Times</t>
   </si>
@@ -91,16 +92,111 @@
   </si>
   <si>
     <t>(N)</t>
+  </si>
+  <si>
+    <t>Notes: Conducted two-sided t-tests between averages times of each category and "Market Rate" category. Statistical significance represented by: *** (&lt;0.01), ** (&lt;0.05), * (&lt;0.1)</t>
+  </si>
+  <si>
+    <t>0.25***</t>
+  </si>
+  <si>
+    <t>0.1***</t>
+  </si>
+  <si>
+    <t>0.13***</t>
+  </si>
+  <si>
+    <t>0.15**</t>
+  </si>
+  <si>
+    <t>0.02***</t>
+  </si>
+  <si>
+    <t>0.05***</t>
+  </si>
+  <si>
+    <t>0.06***</t>
+  </si>
+  <si>
+    <t>0.03***</t>
+  </si>
+  <si>
+    <t>0.04***</t>
+  </si>
+  <si>
+    <t>0.29***</t>
+  </si>
+  <si>
+    <t>0.16***</t>
+  </si>
+  <si>
+    <t>0.19***</t>
+  </si>
+  <si>
+    <t>Within Area Plan</t>
+  </si>
+  <si>
+    <t>Outside Area Plan</t>
+  </si>
+  <si>
+    <t>2.75***</t>
+  </si>
+  <si>
+    <t>(383)</t>
+  </si>
+  <si>
+    <t>(706)</t>
+  </si>
+  <si>
+    <t>(235)</t>
+  </si>
+  <si>
+    <t>(415)</t>
+  </si>
+  <si>
+    <t>(262)</t>
+  </si>
+  <si>
+    <t>(459)</t>
+  </si>
+  <si>
+    <t>5.22***</t>
+  </si>
+  <si>
+    <t>0.87***</t>
+  </si>
+  <si>
+    <t>0.49***</t>
+  </si>
+  <si>
+    <t>0.61***</t>
+  </si>
+  <si>
+    <t>1.8***</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
@@ -113,7 +209,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -141,9 +237,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -154,9 +287,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -164,8 +294,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="29">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -495,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E11"/>
+  <dimension ref="A2:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -509,19 +670,19 @@
     <col min="5" max="5" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="16" thickBot="1"/>
+    <row r="2" spans="1:5" ht="7" customHeight="1" thickBot="1"/>
     <row r="3" spans="1:5">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -543,19 +704,19 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -577,19 +738,19 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -611,19 +772,19 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -645,26 +806,418 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" thickBot="1">
-      <c r="A11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="7" customHeight="1"/>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="7" customHeight="1" thickBot="1"/>
+    <row r="20" spans="1:5">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16" thickBot="1">
+      <c r="A28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="7" customHeight="1"/>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="B5:E5 B7:E11" numberStoredAsText="1"/>
+    <ignoredError sqref="B5:E5 B7:E11 B22:E22 B24:E24 B26:E26 B28:E28" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" ht="7" customHeight="1" thickBot="1"/>
+    <row r="3" spans="1:3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.32</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3.97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16" thickBot="1">
+      <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="7" customHeight="1"/>
+    <row r="14" spans="1:3" ht="7" customHeight="1" thickBot="1"/>
+    <row r="15" spans="1:3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16" thickBot="1">
+      <c r="A23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="7" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="B5:C9 B11:C11 C10 B17:C17 B19:C19 B21:C21 B23:C23" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>